<commit_message>
Did some timing on laptop
</commit_message>
<xml_diff>
--- a/Timing.xlsx
+++ b/Timing.xlsx
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,17 +604,17 @@
       </c>
       <c r="B2" s="6">
         <f>E12</f>
-        <v>0</v>
+        <v>2.3297366666666668E-4</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6">
         <f>E22</f>
-        <v>0</v>
+        <v>2.7834933333333332E-4</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6">
         <f>E22</f>
-        <v>0</v>
+        <v>2.7834933333333332E-4</v>
       </c>
       <c r="G2" s="7"/>
     </row>
@@ -624,17 +625,17 @@
       </c>
       <c r="B3" s="6">
         <f>E13</f>
-        <v>0</v>
+        <v>2.8850766666666666E-4</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6">
         <f>E23</f>
-        <v>0</v>
+        <v>3.6706833333333334E-4</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6">
         <f>E23</f>
-        <v>0</v>
+        <v>3.6706833333333334E-4</v>
       </c>
       <c r="G3" s="7"/>
     </row>
@@ -645,7 +646,7 @@
       </c>
       <c r="B4" s="6">
         <f>E14</f>
-        <v>0</v>
+        <v>9.2557333333333336E-5</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6">
@@ -666,17 +667,17 @@
       </c>
       <c r="B5" s="6">
         <f>E15</f>
-        <v>0</v>
+        <v>3.2237033333333337E-4</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6">
         <f>E25</f>
-        <v>0</v>
+        <v>3.5329799999999999E-4</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
         <f>E25</f>
-        <v>0</v>
+        <v>3.5329799999999999E-4</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -732,50 +733,84 @@
       <c r="A12" s="5">
         <v>1000000</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="6">
+        <v>2.5261400000000002E-4</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2.1739700000000001E-4</v>
+      </c>
+      <c r="D12" s="17">
+        <v>2.2891E-4</v>
+      </c>
+      <c r="E12" s="7">
+        <f>(B12+C12+D12)/3</f>
+        <v>2.3297366666666668E-4</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <f>A12*2</f>
         <v>2000000</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="6">
+        <v>2.3839099999999999E-4</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3.5691E-4</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.7022199999999998E-4</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" ref="E13:E16" si="1">(B13+C13+D13)/3</f>
+        <v>2.8850766666666666E-4</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <f>A13*2</f>
         <v>4000000</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6">
+        <v>2.7767200000000002E-4</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>9.2557333333333336E-5</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
-        <f>A14*2</f>
-        <v>8000000</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+        <v>10000000</v>
+      </c>
+      <c r="B15" s="17">
+        <v>3.1492100000000002E-4</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3.0611599999999999E-4</v>
+      </c>
+      <c r="D15" s="17">
+        <v>3.4607399999999998E-4</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
+        <v>3.2237033333333337E-4</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <f>A15*2</f>
-        <v>16000000</v>
+        <v>20000000</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
@@ -807,50 +842,82 @@
       <c r="A22" s="5">
         <v>1000000</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="B22" s="6">
+        <v>3.5420100000000001E-4</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1.6524899999999999E-4</v>
+      </c>
+      <c r="D22" s="17">
+        <v>3.15598E-4</v>
+      </c>
+      <c r="E22" s="7">
+        <f>(B22+C22+D22)/3</f>
+        <v>2.7834933333333332E-4</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <f>A22*2</f>
         <v>2000000</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="B23" s="6">
+        <v>3.44719E-4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>3.98222E-4</v>
+      </c>
+      <c r="D23" s="6">
+        <v>3.5826400000000001E-4</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" ref="E23:E26" si="2">(B23+C23+D23)/3</f>
+        <v>3.6706833333333334E-4</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
-        <f t="shared" ref="A24:A26" si="1">A23*2</f>
+        <f t="shared" ref="A24:A26" si="3">A23*2</f>
         <v>4000000</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
-        <f t="shared" si="1"/>
-        <v>8000000</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
+        <v>10000000</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2.2620100000000001E-4</v>
+      </c>
+      <c r="C25" s="6">
+        <v>3.9280400000000002E-4</v>
+      </c>
+      <c r="D25" s="17">
+        <v>4.4088900000000003E-4</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="2"/>
+        <v>3.5329799999999999E-4</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
-        <f t="shared" si="1"/>
-        <v>16000000</v>
+        <f t="shared" si="3"/>
+        <v>20000000</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
@@ -882,50 +949,82 @@
       <c r="A32" s="5">
         <v>1000000</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
+      <c r="B32" s="6">
+        <v>1.17841E-4</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1.02265E-4</v>
+      </c>
+      <c r="D32" s="17">
+        <v>1.2190500000000001E-4</v>
+      </c>
+      <c r="E32" s="7">
+        <f>(B32+C32+D32)/3</f>
+        <v>1.1400366666666668E-4</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <f>A32*2</f>
         <v>2000000</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
+      <c r="B33" s="6">
+        <v>1.32063E-4</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1.4019E-4</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.4696300000000001E-4</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" ref="E33:E36" si="4">(B33+C33+D33)/3</f>
+        <v>1.3973866666666665E-4</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <f t="shared" ref="A34:A36" si="2">A33*2</f>
+        <f t="shared" ref="A34:A36" si="5">A33*2</f>
         <v>4000000</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
-        <f t="shared" si="2"/>
-        <v>8000000</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
+        <v>10000000</v>
+      </c>
+      <c r="B35" s="6">
+        <v>2.35682E-4</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1.53058E-4</v>
+      </c>
+      <c r="D35" s="17">
+        <v>2.32296E-4</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="4"/>
+        <v>2.0701199999999999E-4</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="8">
-        <f t="shared" si="2"/>
-        <v>16000000</v>
+        <f t="shared" si="5"/>
+        <v>20000000</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
+      <c r="E36" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>